<commit_message>
fixed preprocessing error (abstract field overwritten with keywords field) and clean up duplicate data and wrong coloring.
</commit_message>
<xml_diff>
--- a/assets/data/MAXQDA24 Code Matrix Browser.xlsx
+++ b/assets/data/MAXQDA24 Code Matrix Browser.xlsx
@@ -180,7 +180,7 @@
     <t>Set Size - Claimed &gt; Millions or More</t>
   </si>
   <si>
-    <t>Set Size - Claimed &gt; not specified</t>
+    <t>Set Size - Claimed &gt; Not Specified</t>
   </si>
   <si>
     <t>Set Size - Confirmed</t>
@@ -4781,8 +4781,8 @@
       <c r="AD22" s="3">
         <v>0</v>
       </c>
-      <c r="AE22" s="4">
-        <v>1</v>
+      <c r="AE22" s="3">
+        <v>0</v>
       </c>
       <c r="AF22" s="3">
         <v>0</v>
@@ -4884,7 +4884,7 @@
         <v>0</v>
       </c>
       <c r="BM22" s="5">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23">
@@ -5915,8 +5915,8 @@
       <c r="N28" s="3">
         <v>0</v>
       </c>
-      <c r="O28" s="3">
-        <v>0</v>
+      <c r="O28" s="4">
+        <v>1</v>
       </c>
       <c r="P28" s="4">
         <v>1</v>
@@ -6066,7 +6066,7 @@
         <v>0</v>
       </c>
       <c r="BM28" s="5">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29">
@@ -6704,7 +6704,7 @@
         <v>1</v>
       </c>
       <c r="O32" s="5">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P32" s="5">
         <v>8</v>
@@ -6752,7 +6752,7 @@
         <v>0</v>
       </c>
       <c r="AE32" s="5">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AF32" s="5">
         <v>6</v>

</xml_diff>